<commit_message>
save learnable network to disk
</commit_message>
<xml_diff>
--- a/Data/Predictions/Graph Neural Network/exclude_previous_rating_model_1_predictions.xlsx
+++ b/Data/Predictions/Graph Neural Network/exclude_previous_rating_model_1_predictions.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2872,7 +2872,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>CCC</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3824,7 +3824,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4266,7 +4266,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4759,7 +4759,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -5065,7 +5065,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -5099,7 +5099,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -5354,7 +5354,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -5558,7 +5558,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -5626,7 +5626,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -5830,7 +5830,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -5915,7 +5915,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -6034,7 +6034,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -6272,7 +6272,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -6357,7 +6357,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
@@ -6425,7 +6425,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
@@ -6442,7 +6442,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
@@ -6595,7 +6595,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -6663,7 +6663,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -6680,7 +6680,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
@@ -6816,7 +6816,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
@@ -6952,7 +6952,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
@@ -7003,7 +7003,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -7020,7 +7020,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -7054,7 +7054,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>BBB</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
@@ -7173,7 +7173,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>CCC</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -7190,7 +7190,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
@@ -7224,7 +7224,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
@@ -7241,7 +7241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
@@ -7275,7 +7275,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>BBB</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">

</xml_diff>